<commit_message>
Location Results Page added
</commit_message>
<xml_diff>
--- a/TripAdvisorAutomation/src/test/resources/testdata/TestData.xlsx
+++ b/TripAdvisorAutomation/src/test/resources/testdata/TestData.xlsx
@@ -3,21 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cognizant\Learning\git2\TripAdvisorAutomation\TripAdvisorAutomation\resources\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42E25C7-27F4-479F-91DD-CA4974EBE2BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0BFD18E2-E4DA-4E35-A597-CD7B90364277}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3168" yWindow="3168" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17304" windowHeight="12312" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
-    <sheet name="HolidayHomesTest" sheetId="2" r:id="rId2"/>
-    <sheet name="CruisesTest" sheetId="3" r:id="rId3"/>
+    <sheet name="HolidayHomesTest" sheetId="2" r:id="rId1"/>
+    <sheet name="CruisesTest" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:K20"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -375,20 +370,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4F29373-B20E-4CD5-8B0B-B41C4E1609FC}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -413,12 +394,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32102D69-645A-4640-A840-44DD827D8ECD}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added input from Excel
</commit_message>
<xml_diff>
--- a/TripAdvisorAutomation/src/test/resources/testdata/TestData.xlsx
+++ b/TripAdvisorAutomation/src/test/resources/testdata/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cognizant\Learning\git2\TripAdvisorAutomation\TripAdvisorAutomation\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EBAAB6-4C02-430E-92B3-6DE525FE0708}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF924406-FD26-4E51-B881-C1EB62CE5239}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3168" yWindow="3168" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3168" yWindow="3168" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HolidayHomesTest" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Location</t>
   </si>
@@ -50,6 +50,15 @@
   </si>
   <si>
     <t>MSC Armonia</t>
+  </si>
+  <si>
+    <t>Sort By</t>
+  </si>
+  <si>
+    <t>Guest No</t>
+  </si>
+  <si>
+    <t>Traveller Rating</t>
   </si>
 </sst>
 </file>
@@ -381,22 +390,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -408,7 +434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051A3FDE-4415-4BB5-A72E-EA831656C515}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>